<commit_message>
update laporan & journal
</commit_message>
<xml_diff>
--- a/daftar hadir.xlsx
+++ b/daftar hadir.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CV Pixel Dev Intern\LAPORAN CV PIXEL DEV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96746A62-AFBE-44DA-B1BC-33B85842F1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A287A9-C607-4174-95F8-62D6CB3515FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,7 +171,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_([$Rp-421]* #,##0_);_([$Rp-421]* \(#,##0\);_([$Rp-421]* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +236,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="2"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -361,7 +368,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -426,17 +433,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -729,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="116" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,124 +752,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
     </row>
     <row r="2" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="28"/>
-      <c r="Z2" s="28"/>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="28"/>
-      <c r="AE2" s="28"/>
-      <c r="AF2" s="28"/>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="29"/>
+      <c r="AA2" s="29"/>
+      <c r="AB2" s="29"/>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="29"/>
+      <c r="AH2" s="29"/>
     </row>
     <row r="3" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="28"/>
-      <c r="AA3" s="28"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="28"/>
-      <c r="AD3" s="28"/>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="28"/>
-      <c r="AG3" s="28"/>
-      <c r="AH3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29"/>
+      <c r="W3" s="29"/>
+      <c r="X3" s="29"/>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="29"/>
+      <c r="AB3" s="29"/>
+      <c r="AC3" s="29"/>
+      <c r="AD3" s="29"/>
+      <c r="AE3" s="29"/>
+      <c r="AF3" s="29"/>
+      <c r="AG3" s="29"/>
+      <c r="AH3" s="29"/>
     </row>
     <row r="4" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1052,89 +1062,89 @@
       <c r="AH8" s="4"/>
     </row>
     <row r="9" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="29"/>
-      <c r="X9" s="29"/>
-      <c r="Y9" s="29"/>
-      <c r="Z9" s="29"/>
-      <c r="AA9" s="29"/>
-      <c r="AB9" s="29"/>
-      <c r="AC9" s="29"/>
-      <c r="AD9" s="29"/>
-      <c r="AE9" s="29"/>
-      <c r="AF9" s="29"/>
-      <c r="AG9" s="29"/>
-      <c r="AH9" s="29"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="30"/>
+      <c r="W9" s="30"/>
+      <c r="X9" s="30"/>
+      <c r="Y9" s="30"/>
+      <c r="Z9" s="30"/>
+      <c r="AA9" s="30"/>
+      <c r="AB9" s="30"/>
+      <c r="AC9" s="30"/>
+      <c r="AD9" s="30"/>
+      <c r="AE9" s="30"/>
+      <c r="AF9" s="30"/>
+      <c r="AG9" s="30"/>
+      <c r="AH9" s="30"/>
     </row>
     <row r="10" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="30"/>
-      <c r="W10" s="30"/>
-      <c r="X10" s="30"/>
-      <c r="Y10" s="30"/>
-      <c r="Z10" s="30"/>
-      <c r="AA10" s="30"/>
-      <c r="AB10" s="30"/>
-      <c r="AC10" s="30"/>
-      <c r="AD10" s="30"/>
-      <c r="AE10" s="30"/>
-      <c r="AF10" s="30"/>
-      <c r="AG10" s="30"/>
-      <c r="AH10" s="30"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="32"/>
+      <c r="X10" s="32"/>
+      <c r="Y10" s="32"/>
+      <c r="Z10" s="32"/>
+      <c r="AA10" s="32"/>
+      <c r="AB10" s="32"/>
+      <c r="AC10" s="32"/>
+      <c r="AD10" s="32"/>
+      <c r="AE10" s="32"/>
+      <c r="AF10" s="32"/>
+      <c r="AG10" s="32"/>
+      <c r="AH10" s="32"/>
     </row>
     <row r="11" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="1">
         <v>1</v>
       </c>
@@ -1425,10 +1435,10 @@
       <c r="AA16" s="5"/>
       <c r="AB16" s="5"/>
       <c r="AC16" s="13"/>
-      <c r="AD16" s="5"/>
-      <c r="AE16" s="5"/>
-      <c r="AF16" s="5"/>
-      <c r="AG16" s="5"/>
+      <c r="AD16" s="28"/>
+      <c r="AE16" s="24"/>
+      <c r="AF16" s="24"/>
+      <c r="AG16" s="24"/>
       <c r="AH16" s="14"/>
     </row>
     <row r="17" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
@@ -1440,7 +1450,7 @@
         <v>20</v>
       </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="22"/>
       <c r="G17" s="23"/>
       <c r="H17" s="23"/>

</xml_diff>